<commit_message>
Edit README.md and csv
</commit_message>
<xml_diff>
--- a/data/efficient_shopping_optimizer_data.xlsx
+++ b/data/efficient_shopping_optimizer_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eunjaeyu/Developer/portfolio/efficient-shopping-optimizer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FC158C-455E-064D-8A24-4CCC0EED29B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBB79C0-5803-5744-A6B9-F2E900A9C6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16600" xr2:uid="{2E35BC18-434B-7544-9700-4F3218D8AD44}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16580" xr2:uid="{2E35BC18-434B-7544-9700-4F3218D8AD44}"/>
   </bookViews>
   <sheets>
     <sheet name="efficient_shopping_optimizer_da" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="82">
   <si>
     <t>category</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>snack</t>
-  </si>
-  <si>
-    <t>Chieck Breast</t>
   </si>
   <si>
     <t>Almond</t>
@@ -675,7 +672,7 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,24 +718,24 @@
         <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -766,16 +763,16 @@
         <v>7.1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N2" s="1">
         <f xml:space="preserve"> G2/E2</f>
@@ -795,7 +792,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -823,16 +820,16 @@
         <v>2.6</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N3" s="1">
         <f t="shared" ref="N3:N40" si="1" xml:space="preserve"> G3/E3</f>
@@ -889,7 +886,7 @@
         <v>22</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" si="1"/>
@@ -946,7 +943,7 @@
         <v>22</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="1"/>
@@ -966,7 +963,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -994,7 +991,7 @@
         <v>2.7</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>9</v>
@@ -1003,7 +1000,7 @@
         <v>22</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" si="1"/>
@@ -1023,7 +1020,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1051,7 +1048,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>9</v>
@@ -1060,7 +1057,7 @@
         <v>22</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="1"/>
@@ -1117,7 +1114,7 @@
         <v>22</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="1"/>
@@ -1174,7 +1171,7 @@
         <v>21</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="1"/>
@@ -1231,7 +1228,7 @@
         <v>22</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="1"/>
@@ -1288,7 +1285,7 @@
         <v>22</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N11" s="1">
         <f t="shared" si="1"/>
@@ -1308,7 +1305,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -1336,7 +1333,7 @@
         <v>1.7</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>9</v>
@@ -1345,7 +1342,7 @@
         <v>22</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="1"/>
@@ -1402,7 +1399,7 @@
         <v>22</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N13" s="1">
         <f t="shared" si="1"/>
@@ -1422,7 +1419,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -1450,7 +1447,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>9</v>
@@ -1459,7 +1456,7 @@
         <v>22</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N14" s="1">
         <f t="shared" si="1"/>
@@ -1479,7 +1476,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
@@ -1516,7 +1513,7 @@
         <v>21</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N15" s="1">
         <f t="shared" si="1"/>
@@ -1536,7 +1533,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -1573,7 +1570,7 @@
         <v>21</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N16" s="1">
         <f t="shared" si="1"/>
@@ -1593,7 +1590,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
@@ -1621,7 +1618,7 @@
         <v>7.1</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>19</v>
@@ -1630,7 +1627,7 @@
         <v>22</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N17" s="1">
         <f t="shared" si="1"/>
@@ -1687,7 +1684,7 @@
         <v>22</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N18" s="1">
         <f t="shared" si="1"/>
@@ -1744,7 +1741,7 @@
         <v>22</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N19" s="1">
         <f t="shared" si="1"/>
@@ -1764,7 +1761,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -1792,7 +1789,7 @@
         <v>2.7</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>19</v>
@@ -1801,7 +1798,7 @@
         <v>22</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N20" s="1">
         <f t="shared" si="1"/>
@@ -1821,7 +1818,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -1849,7 +1846,7 @@
         <v>3</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>19</v>
@@ -1858,7 +1855,7 @@
         <v>22</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N21" s="1">
         <f t="shared" si="1"/>
@@ -1915,7 +1912,7 @@
         <v>22</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N22" s="1">
         <f t="shared" si="1"/>
@@ -1933,7 +1930,7 @@
         <v>5</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
@@ -1975,7 +1972,7 @@
         <v>21</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N23" s="1">
         <f t="shared" si="1"/>
@@ -2032,7 +2029,7 @@
         <v>22</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N24" s="1">
         <f t="shared" si="1"/>
@@ -2052,7 +2049,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
@@ -2089,7 +2086,7 @@
         <v>21</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N25" s="1">
         <f t="shared" si="1"/>
@@ -2146,7 +2143,7 @@
         <v>22</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N26" s="1">
         <f t="shared" si="1"/>
@@ -2203,7 +2200,7 @@
         <v>22</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N27" s="1">
         <f t="shared" si="1"/>
@@ -2260,7 +2257,7 @@
         <v>22</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N28" s="1">
         <f t="shared" si="1"/>
@@ -2280,7 +2277,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -2308,7 +2305,7 @@
         <v>1.7</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>19</v>
@@ -2317,7 +2314,7 @@
         <v>22</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N29" s="1">
         <f t="shared" si="1"/>
@@ -2374,7 +2371,7 @@
         <v>22</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N30" s="1">
         <f t="shared" si="1"/>
@@ -2394,7 +2391,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
@@ -2431,7 +2428,7 @@
         <v>21</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N31" s="1">
         <f t="shared" si="1"/>
@@ -2451,7 +2448,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
@@ -2488,7 +2485,7 @@
         <v>22</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N32" s="1">
         <f t="shared" si="1"/>
@@ -2508,7 +2505,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
@@ -2536,7 +2533,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>19</v>
@@ -2545,7 +2542,7 @@
         <v>22</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N33" s="1">
         <f t="shared" si="1"/>
@@ -2602,7 +2599,7 @@
         <v>22</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N34" s="1">
         <f xml:space="preserve"> G34/E34</f>
@@ -2659,7 +2656,7 @@
         <v>22</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N35" s="1">
         <f t="shared" si="1"/>
@@ -2716,7 +2713,7 @@
         <v>22</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N36" s="1">
         <f t="shared" si="1"/>
@@ -2773,7 +2770,7 @@
         <v>22</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N37" s="1">
         <f t="shared" si="1"/>
@@ -2793,7 +2790,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -2830,7 +2827,7 @@
         <v>22</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N38" s="1">
         <f t="shared" si="1"/>
@@ -2850,7 +2847,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -2887,7 +2884,7 @@
         <v>21</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N39" s="1">
         <f t="shared" si="1"/>
@@ -2907,7 +2904,7 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
@@ -2944,7 +2941,7 @@
         <v>21</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N40" s="1">
         <f t="shared" si="1"/>

</xml_diff>